<commit_message>
added more validation tracks
</commit_message>
<xml_diff>
--- a/validation/analysis.xlsx
+++ b/validation/analysis.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\engs1397\Documents\Teaching\4Yprojects\2016 Jamieson Brynes\data\validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\engs1397\Documents\Teaching\4Yprojects\2016 Jamieson Brynes\data\DataSet\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7560" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="files" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
   <si>
     <t>filename</t>
   </si>
@@ -106,6 +106,39 @@
   </si>
   <si>
     <t>hw accuracy</t>
+  </si>
+  <si>
+    <t>stepcounter_1503572116339.csv</t>
+  </si>
+  <si>
+    <t>stepcounter_1503572296043.csv</t>
+  </si>
+  <si>
+    <t>stepcounter_1503572567249.csv</t>
+  </si>
+  <si>
+    <t>stepcounter_1503572776963.csv</t>
+  </si>
+  <si>
+    <t>stepcounter_1503573010286.csv</t>
+  </si>
+  <si>
+    <t>stepcounter_1503573264996.csv</t>
+  </si>
+  <si>
+    <t>neck pouch</t>
+  </si>
+  <si>
+    <t>armband</t>
+  </si>
+  <si>
+    <t>purse</t>
+  </si>
+  <si>
+    <t>stepcounter_1503573489803.csv</t>
+  </si>
+  <si>
+    <t>frestyle</t>
   </si>
 </sst>
 </file>
@@ -434,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,7 +538,7 @@
         <v>400</v>
       </c>
       <c r="I2" s="1">
-        <f>ABS(E2-F2) / F2</f>
+        <f t="shared" ref="I2:I14" si="0">ABS(E2-F2) / F2</f>
         <v>0.16417910447761194</v>
       </c>
       <c r="J2" s="2">
@@ -544,19 +577,19 @@
         <v>401</v>
       </c>
       <c r="I3" s="1">
-        <f>ABS(E3-F3) / F3</f>
+        <f t="shared" si="0"/>
         <v>0.15920398009950248</v>
       </c>
       <c r="J3" s="2">
-        <f t="shared" ref="J3:J7" si="0">1-I3</f>
+        <f t="shared" ref="J3:J14" si="1">1-I3</f>
         <v>0.84079601990049757</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L7" si="1">ABS(G3-F3)/F3</f>
+        <f t="shared" ref="L3:L14" si="2">ABS(G3-F3)/F3</f>
         <v>2.4875621890547263E-3</v>
       </c>
       <c r="M3" s="2">
-        <f t="shared" ref="M3:M7" si="2" xml:space="preserve"> 1 -L3</f>
+        <f t="shared" ref="M3:M14" si="3" xml:space="preserve"> 1 -L3</f>
         <v>0.99751243781094523</v>
       </c>
     </row>
@@ -583,19 +616,19 @@
         <v>309</v>
       </c>
       <c r="I4" s="1">
-        <f>ABS(E4-F4) / F4</f>
+        <f t="shared" si="0"/>
         <v>0.26490066225165565</v>
       </c>
       <c r="J4" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.73509933774834435</v>
       </c>
       <c r="L4" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.3178807947019868E-2</v>
       </c>
       <c r="M4" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.97682119205298013</v>
       </c>
     </row>
@@ -622,19 +655,19 @@
         <v>257</v>
       </c>
       <c r="I5" s="1">
-        <f>ABS(E5-F5) / F5</f>
+        <f t="shared" si="0"/>
         <v>0.18431372549019609</v>
       </c>
       <c r="J5" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.81568627450980391</v>
       </c>
       <c r="L5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.8431372549019607E-3</v>
       </c>
       <c r="M5" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.99215686274509807</v>
       </c>
     </row>
@@ -661,19 +694,19 @@
         <v>313</v>
       </c>
       <c r="I6" s="1">
-        <f>ABS(E6-F6) / F6</f>
+        <f t="shared" si="0"/>
         <v>6.8111455108359129E-2</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.93188854489164086</v>
       </c>
       <c r="L6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.0959752321981424E-2</v>
       </c>
       <c r="M6" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.96904024767801855</v>
       </c>
     </row>
@@ -700,20 +733,290 @@
         <v>474</v>
       </c>
       <c r="I7" s="1">
-        <f>ABS(E7-F7) / F7</f>
+        <f t="shared" si="0"/>
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="J7" s="2">
+        <f t="shared" si="1"/>
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="L7" s="1">
+        <f t="shared" si="2"/>
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" si="3"/>
+        <v>0.73599999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>271</v>
+      </c>
+      <c r="F8">
+        <v>300</v>
+      </c>
+      <c r="G8">
+        <v>299</v>
+      </c>
+      <c r="I8" s="1">
         <f t="shared" si="0"/>
-        <v>0.95199999999999996</v>
-      </c>
-      <c r="L7" s="1">
+        <v>9.6666666666666665E-2</v>
+      </c>
+      <c r="J8" s="2">
         <f t="shared" si="1"/>
-        <v>0.26400000000000001</v>
-      </c>
-      <c r="M7" s="2">
+        <v>0.90333333333333332</v>
+      </c>
+      <c r="L8" s="1">
         <f t="shared" si="2"/>
-        <v>0.73599999999999999</v>
+        <v>3.3333333333333335E-3</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="3"/>
+        <v>0.9966666666666667</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <v>356</v>
+      </c>
+      <c r="F9">
+        <v>383</v>
+      </c>
+      <c r="G9">
+        <v>380</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="0"/>
+        <v>7.0496083550913843E-2</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="1"/>
+        <v>0.92950391644908614</v>
+      </c>
+      <c r="L9" s="1">
+        <f t="shared" si="2"/>
+        <v>7.832898172323759E-3</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="3"/>
+        <v>0.9921671018276762</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10">
+        <v>240</v>
+      </c>
+      <c r="F10">
+        <v>290</v>
+      </c>
+      <c r="G10">
+        <v>296</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.17241379310344829</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="1"/>
+        <v>0.82758620689655171</v>
+      </c>
+      <c r="L10" s="1">
+        <f t="shared" si="2"/>
+        <v>2.0689655172413793E-2</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="3"/>
+        <v>0.97931034482758617</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11">
+        <v>235</v>
+      </c>
+      <c r="F11">
+        <v>292</v>
+      </c>
+      <c r="G11">
+        <v>295</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1952054794520548</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.8047945205479452</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" si="2"/>
+        <v>1.0273972602739725E-2</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="3"/>
+        <v>0.98972602739726023</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12">
+        <v>301</v>
+      </c>
+      <c r="F12">
+        <v>370</v>
+      </c>
+      <c r="G12">
+        <v>364</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1864864864864865</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="1"/>
+        <v>0.81351351351351353</v>
+      </c>
+      <c r="L12" s="1">
+        <f t="shared" si="2"/>
+        <v>1.6216216216216217E-2</v>
+      </c>
+      <c r="M12" s="2">
+        <f t="shared" si="3"/>
+        <v>0.98378378378378373</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13">
+        <v>222</v>
+      </c>
+      <c r="F13">
+        <v>331</v>
+      </c>
+      <c r="G13">
+        <v>328</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="0"/>
+        <v>0.32930513595166161</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="1"/>
+        <v>0.67069486404833834</v>
+      </c>
+      <c r="L13" s="1">
+        <f t="shared" si="2"/>
+        <v>9.0634441087613302E-3</v>
+      </c>
+      <c r="M13" s="2">
+        <f t="shared" si="3"/>
+        <v>0.99093655589123864</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14">
+        <v>455</v>
+      </c>
+      <c r="F14">
+        <v>689</v>
+      </c>
+      <c r="G14">
+        <v>685</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33962264150943394</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="1"/>
+        <v>0.66037735849056611</v>
+      </c>
+      <c r="L14" s="1">
+        <f t="shared" si="2"/>
+        <v>5.8055152394775036E-3</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="3"/>
+        <v>0.99419448476052252</v>
       </c>
     </row>
   </sheetData>
@@ -723,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,6 +1117,90 @@
         <v>0.16478433942251997</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="2">
+        <f>AVERAGE(files!J8:J9)</f>
+        <v>0.91641862489120973</v>
+      </c>
+      <c r="C5" s="2">
+        <f>_xlfn.STDEV.S(files!J8:J9)</f>
+        <v>1.8505396788754985E-2</v>
+      </c>
+      <c r="E5" s="2">
+        <f>AVERAGE(files!M8:M9)</f>
+        <v>0.99441688424717145</v>
+      </c>
+      <c r="F5" s="2">
+        <f>_xlfn.STDEV.S(files!M8:M9)</f>
+        <v>3.1816728100387383E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="2">
+        <f>AVERAGE(files!J10:J11)</f>
+        <v>0.81619036372224851</v>
+      </c>
+      <c r="C6" s="2">
+        <f>_xlfn.STDEV.S(files!J10:J11)</f>
+        <v>1.6116155971776527E-2</v>
+      </c>
+      <c r="E6" s="2">
+        <f>AVERAGE(files!M10:M11)</f>
+        <v>0.98451818611242325</v>
+      </c>
+      <c r="F6" s="2">
+        <f>_xlfn.STDEV.S(files!M10:M11)</f>
+        <v>7.3649997757030579E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="2">
+        <f>AVERAGE(files!J12:J13)</f>
+        <v>0.74210418878092588</v>
+      </c>
+      <c r="C7" s="2">
+        <f>_xlfn.STDEV.S(files!J12:J13)</f>
+        <v>0.10098803551672987</v>
+      </c>
+      <c r="E7" s="2">
+        <f>AVERAGE(files!M12:M13)</f>
+        <v>0.98736016983751118</v>
+      </c>
+      <c r="F7" s="2">
+        <f>_xlfn.STDEV.S(files!M12:M13)</f>
+        <v>5.0577736614633578E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="2">
+        <f>AVERAGE(files!J14:J14)</f>
+        <v>0.66037735849056611</v>
+      </c>
+      <c r="C8" s="2" t="e">
+        <f>_xlfn.STDEV.S(files!J14:J14)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E8" s="2">
+        <f>AVERAGE(files!M14:M14)</f>
+        <v>0.99419448476052252</v>
+      </c>
+      <c r="F8" s="2" t="e">
+        <f>_xlfn.STDEV.S(files!M14:M14)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
udpated data set with DB and validation traces
</commit_message>
<xml_diff>
--- a/validation/analysis.xlsx
+++ b/validation/analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7560" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7560"/>
   </bookViews>
   <sheets>
     <sheet name="files" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>filename</t>
   </si>
@@ -45,24 +45,6 @@
     <t>algo</t>
   </si>
   <si>
-    <t>stepcounter_1503502498728.csv</t>
-  </si>
-  <si>
-    <t>stepcounter_1503502721170.csv</t>
-  </si>
-  <si>
-    <t>stepcounter_1503502959664.csv</t>
-  </si>
-  <si>
-    <t>stepcounter_1503503150186.csv</t>
-  </si>
-  <si>
-    <t>stepcounter_1503503318306.csv</t>
-  </si>
-  <si>
-    <t>stepcounter_1503503518075.csv</t>
-  </si>
-  <si>
     <t>dario</t>
   </si>
   <si>
@@ -108,24 +90,6 @@
     <t>hw accuracy</t>
   </si>
   <si>
-    <t>stepcounter_1503572116339.csv</t>
-  </si>
-  <si>
-    <t>stepcounter_1503572296043.csv</t>
-  </si>
-  <si>
-    <t>stepcounter_1503572567249.csv</t>
-  </si>
-  <si>
-    <t>stepcounter_1503572776963.csv</t>
-  </si>
-  <si>
-    <t>stepcounter_1503573010286.csv</t>
-  </si>
-  <si>
-    <t>stepcounter_1503573264996.csv</t>
-  </si>
-  <si>
     <t>neck pouch</t>
   </si>
   <si>
@@ -135,10 +99,31 @@
     <t>purse</t>
   </si>
   <si>
-    <t>stepcounter_1503573489803.csv</t>
-  </si>
-  <si>
     <t>frestyle</t>
+  </si>
+  <si>
+    <t>stepcounter_1505740246677</t>
+  </si>
+  <si>
+    <t>stepcounter_1505741047626</t>
+  </si>
+  <si>
+    <t>stepcounter_1505741332224</t>
+  </si>
+  <si>
+    <t>stepcounter_1505741614989</t>
+  </si>
+  <si>
+    <t>stepcounter_1505741827924</t>
+  </si>
+  <si>
+    <t>front_pocket</t>
+  </si>
+  <si>
+    <t>back_pocket</t>
+  </si>
+  <si>
+    <t>stepcounter_1505742017961</t>
   </si>
 </sst>
 </file>
@@ -469,8 +454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,6 +463,7 @@
     <col min="1" max="1" width="33" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -500,524 +486,296 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" t="s">
         <v>20</v>
-      </c>
-      <c r="I1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E2">
-        <v>336</v>
+        <v>313</v>
       </c>
       <c r="F2">
-        <v>402</v>
+        <v>288</v>
       </c>
       <c r="G2">
-        <v>400</v>
+        <v>983</v>
       </c>
       <c r="I2" s="1">
         <f t="shared" ref="I2:I14" si="0">ABS(E2-F2) / F2</f>
-        <v>0.16417910447761194</v>
+        <v>8.6805555555555552E-2</v>
       </c>
       <c r="J2" s="2">
         <f>1-I2</f>
-        <v>0.83582089552238803</v>
+        <v>0.91319444444444442</v>
       </c>
       <c r="L2" s="1">
         <f>ABS(G2-F2)/F2</f>
-        <v>4.9751243781094526E-3</v>
+        <v>2.4131944444444446</v>
       </c>
       <c r="M2" s="2">
         <f xml:space="preserve"> 1 -L2</f>
-        <v>0.99502487562189057</v>
+        <v>-1.4131944444444446</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E3">
-        <v>338</v>
+        <v>297</v>
       </c>
       <c r="F3">
-        <v>402</v>
+        <v>279</v>
       </c>
       <c r="G3">
-        <v>401</v>
+        <v>966</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" si="0"/>
-        <v>0.15920398009950248</v>
+        <f t="shared" ref="I3" si="1">ABS(E3-F3) / F3</f>
+        <v>6.4516129032258063E-2</v>
       </c>
       <c r="J3" s="2">
-        <f t="shared" ref="J3:J14" si="1">1-I3</f>
-        <v>0.84079601990049757</v>
+        <f>1-I3</f>
+        <v>0.93548387096774199</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L14" si="2">ABS(G3-F3)/F3</f>
-        <v>2.4875621890547263E-3</v>
+        <f>ABS(G3-F3)/F3</f>
+        <v>2.4623655913978495</v>
       </c>
       <c r="M3" s="2">
-        <f t="shared" ref="M3:M14" si="3" xml:space="preserve"> 1 -L3</f>
-        <v>0.99751243781094523</v>
+        <f xml:space="preserve"> 1 -L3</f>
+        <v>-1.4623655913978495</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E4">
-        <v>222</v>
+        <v>421</v>
       </c>
       <c r="F4">
-        <v>302</v>
+        <v>346</v>
       </c>
       <c r="G4">
-        <v>309</v>
+        <v>1090</v>
       </c>
       <c r="I4" s="1">
-        <f t="shared" si="0"/>
-        <v>0.26490066225165565</v>
+        <f t="shared" ref="I4" si="2">ABS(E4-F4) / F4</f>
+        <v>0.21676300578034682</v>
       </c>
       <c r="J4" s="2">
-        <f t="shared" si="1"/>
-        <v>0.73509933774834435</v>
+        <f>1-I4</f>
+        <v>0.7832369942196532</v>
       </c>
       <c r="L4" s="1">
-        <f t="shared" si="2"/>
-        <v>2.3178807947019868E-2</v>
+        <f>ABS(G4-F4)/F4</f>
+        <v>2.1502890173410405</v>
       </c>
       <c r="M4" s="2">
-        <f t="shared" si="3"/>
-        <v>0.97682119205298013</v>
+        <f xml:space="preserve"> 1 -L4</f>
+        <v>-1.1502890173410405</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E5">
-        <v>208</v>
+        <v>366</v>
       </c>
       <c r="F5">
-        <v>255</v>
+        <v>286</v>
       </c>
       <c r="G5">
-        <v>257</v>
+        <v>843</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" si="0"/>
-        <v>0.18431372549019609</v>
+        <f t="shared" ref="I5" si="3">ABS(E5-F5) / F5</f>
+        <v>0.27972027972027974</v>
       </c>
       <c r="J5" s="2">
-        <f t="shared" si="1"/>
-        <v>0.81568627450980391</v>
+        <f>1-I5</f>
+        <v>0.7202797202797202</v>
       </c>
       <c r="L5" s="1">
-        <f t="shared" si="2"/>
-        <v>7.8431372549019607E-3</v>
+        <f>ABS(G5-F5)/F5</f>
+        <v>1.9475524475524475</v>
       </c>
       <c r="M5" s="2">
-        <f t="shared" si="3"/>
-        <v>0.99215686274509807</v>
+        <f xml:space="preserve"> 1 -L5</f>
+        <v>-0.9475524475524475</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
       <c r="E6">
-        <v>301</v>
+        <v>350</v>
       </c>
       <c r="F6">
-        <v>323</v>
+        <v>263</v>
       </c>
       <c r="G6">
-        <v>313</v>
+        <v>764</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="0"/>
-        <v>6.8111455108359129E-2</v>
+        <f t="shared" ref="I6:I7" si="4">ABS(E6-F6) / F6</f>
+        <v>0.33079847908745247</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" si="1"/>
-        <v>0.93188854489164086</v>
+        <f t="shared" ref="J6:J7" si="5">1-I6</f>
+        <v>0.66920152091254748</v>
       </c>
       <c r="L6" s="1">
-        <f t="shared" si="2"/>
-        <v>3.0959752321981424E-2</v>
+        <f t="shared" ref="L6:L7" si="6">ABS(G6-F6)/F6</f>
+        <v>1.9049429657794676</v>
       </c>
       <c r="M6" s="2">
-        <f t="shared" si="3"/>
-        <v>0.96904024767801855</v>
+        <f t="shared" ref="M6:M7" si="7" xml:space="preserve"> 1 -L6</f>
+        <v>-0.90494296577946765</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E7">
-        <v>357</v>
+        <v>285</v>
       </c>
       <c r="F7">
-        <v>375</v>
+        <v>266</v>
       </c>
       <c r="G7">
-        <v>474</v>
+        <v>735</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" si="0"/>
-        <v>4.8000000000000001E-2</v>
+        <f t="shared" si="4"/>
+        <v>7.1428571428571425E-2</v>
       </c>
       <c r="J7" s="2">
-        <f t="shared" si="1"/>
-        <v>0.95199999999999996</v>
+        <f t="shared" si="5"/>
+        <v>0.9285714285714286</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" si="2"/>
-        <v>0.26400000000000001</v>
+        <f t="shared" si="6"/>
+        <v>1.763157894736842</v>
       </c>
       <c r="M7" s="2">
-        <f t="shared" si="3"/>
-        <v>0.73599999999999999</v>
+        <f t="shared" si="7"/>
+        <v>-0.76315789473684204</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8">
-        <v>271</v>
-      </c>
-      <c r="F8">
-        <v>300</v>
-      </c>
-      <c r="G8">
-        <v>299</v>
-      </c>
-      <c r="I8" s="1">
-        <f t="shared" si="0"/>
-        <v>9.6666666666666665E-2</v>
-      </c>
-      <c r="J8" s="2">
-        <f t="shared" si="1"/>
-        <v>0.90333333333333332</v>
-      </c>
-      <c r="L8" s="1">
-        <f t="shared" si="2"/>
-        <v>3.3333333333333335E-3</v>
-      </c>
-      <c r="M8" s="2">
-        <f t="shared" si="3"/>
-        <v>0.9966666666666667</v>
-      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="2"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="2"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9">
-        <v>356</v>
-      </c>
-      <c r="F9">
-        <v>383</v>
-      </c>
-      <c r="G9">
-        <v>380</v>
-      </c>
-      <c r="I9" s="1">
-        <f t="shared" si="0"/>
-        <v>7.0496083550913843E-2</v>
-      </c>
-      <c r="J9" s="2">
-        <f t="shared" si="1"/>
-        <v>0.92950391644908614</v>
-      </c>
-      <c r="L9" s="1">
-        <f t="shared" si="2"/>
-        <v>7.832898172323759E-3</v>
-      </c>
-      <c r="M9" s="2">
-        <f t="shared" si="3"/>
-        <v>0.9921671018276762</v>
-      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="2"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10">
-        <v>240</v>
-      </c>
-      <c r="F10">
-        <v>290</v>
-      </c>
-      <c r="G10">
-        <v>296</v>
-      </c>
-      <c r="I10" s="1">
-        <f t="shared" si="0"/>
-        <v>0.17241379310344829</v>
-      </c>
-      <c r="J10" s="2">
-        <f t="shared" si="1"/>
-        <v>0.82758620689655171</v>
-      </c>
-      <c r="L10" s="1">
-        <f t="shared" si="2"/>
-        <v>2.0689655172413793E-2</v>
-      </c>
-      <c r="M10" s="2">
-        <f t="shared" si="3"/>
-        <v>0.97931034482758617</v>
-      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="2"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="2"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11">
-        <v>235</v>
-      </c>
-      <c r="F11">
-        <v>292</v>
-      </c>
-      <c r="G11">
-        <v>295</v>
-      </c>
-      <c r="I11" s="1">
-        <f t="shared" si="0"/>
-        <v>0.1952054794520548</v>
-      </c>
-      <c r="J11" s="2">
-        <f t="shared" si="1"/>
-        <v>0.8047945205479452</v>
-      </c>
-      <c r="L11" s="1">
-        <f t="shared" si="2"/>
-        <v>1.0273972602739725E-2</v>
-      </c>
-      <c r="M11" s="2">
-        <f t="shared" si="3"/>
-        <v>0.98972602739726023</v>
-      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="2"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="2"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12">
-        <v>301</v>
-      </c>
-      <c r="F12">
-        <v>370</v>
-      </c>
-      <c r="G12">
-        <v>364</v>
-      </c>
-      <c r="I12" s="1">
-        <f t="shared" si="0"/>
-        <v>0.1864864864864865</v>
-      </c>
-      <c r="J12" s="2">
-        <f t="shared" si="1"/>
-        <v>0.81351351351351353</v>
-      </c>
-      <c r="L12" s="1">
-        <f t="shared" si="2"/>
-        <v>1.6216216216216217E-2</v>
-      </c>
-      <c r="M12" s="2">
-        <f t="shared" si="3"/>
-        <v>0.98378378378378373</v>
-      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="2"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="2"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13">
-        <v>222</v>
-      </c>
-      <c r="F13">
-        <v>331</v>
-      </c>
-      <c r="G13">
-        <v>328</v>
-      </c>
-      <c r="I13" s="1">
-        <f t="shared" si="0"/>
-        <v>0.32930513595166161</v>
-      </c>
-      <c r="J13" s="2">
-        <f t="shared" si="1"/>
-        <v>0.67069486404833834</v>
-      </c>
-      <c r="L13" s="1">
-        <f t="shared" si="2"/>
-        <v>9.0634441087613302E-3</v>
-      </c>
-      <c r="M13" s="2">
-        <f t="shared" si="3"/>
-        <v>0.99093655589123864</v>
-      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="2"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="2"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14">
-        <v>455</v>
-      </c>
-      <c r="F14">
-        <v>689</v>
-      </c>
-      <c r="G14">
-        <v>685</v>
-      </c>
-      <c r="I14" s="1">
-        <f t="shared" si="0"/>
-        <v>0.33962264150943394</v>
-      </c>
-      <c r="J14" s="2">
-        <f t="shared" si="1"/>
-        <v>0.66037735849056611</v>
-      </c>
-      <c r="L14" s="1">
-        <f t="shared" si="2"/>
-        <v>5.8055152394775036E-3</v>
-      </c>
-      <c r="M14" s="2">
-        <f t="shared" si="3"/>
-        <v>0.99419448476052252</v>
-      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="2"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1028,7 +786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -1039,162 +797,162 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2">
         <f>AVERAGE(files!J2:J3)</f>
-        <v>0.8383084577114428</v>
+        <v>0.92433915770609321</v>
       </c>
       <c r="C2" s="2">
         <f>_xlfn.STDEV.S(files!J2:J3)</f>
-        <v>3.5179441850077616E-3</v>
+        <v>1.5761004643383005E-2</v>
       </c>
       <c r="E2" s="2">
         <f>AVERAGE(files!M2:M3)</f>
-        <v>0.99626865671641784</v>
+        <v>-1.4377800179211471</v>
       </c>
       <c r="F2" s="2">
         <f>_xlfn.STDEV.S(files!M2:M3)</f>
-        <v>1.7589720925038023E-3</v>
+        <v>3.4769251449472821E-2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2">
         <f>AVERAGE(files!J4:J5)</f>
-        <v>0.77539280612907413</v>
+        <v>0.75175835724968665</v>
       </c>
       <c r="C3" s="2">
         <f>_xlfn.STDEV.S(files!J4:J5)</f>
-        <v>5.6983569459079529E-2</v>
+        <v>4.4517515327945741E-2</v>
       </c>
       <c r="E3" s="2">
         <f>AVERAGE(files!M4:M5)</f>
-        <v>0.9844890273990391</v>
+        <v>-1.048920732446744</v>
       </c>
       <c r="F3" s="2">
         <f>_xlfn.STDEV.S(files!M4:M5)</f>
-        <v>1.0843956740440391E-2</v>
+        <v>0.14335640329201385</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2">
         <f>AVERAGE(files!J6:J7)</f>
-        <v>0.94194427244582046</v>
+        <v>0.79888647474198804</v>
       </c>
       <c r="C4" s="2">
         <f>_xlfn.STDEV.S(files!J6:J7)</f>
-        <v>1.4220946286649551E-2</v>
+        <v>0.18340222054132363</v>
       </c>
       <c r="E4" s="2">
         <f>AVERAGE(files!M6:M7)</f>
-        <v>0.85252012383900921</v>
+        <v>-0.83405043025815484</v>
       </c>
       <c r="F4" s="2">
         <f>_xlfn.STDEV.S(files!M6:M7)</f>
-        <v>0.16478433942251997</v>
+        <v>0.10025718520525696</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="2">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="e">
         <f>AVERAGE(files!J8:J9)</f>
-        <v>0.91641862489120973</v>
-      </c>
-      <c r="C5" s="2">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C5" s="2" t="e">
         <f>_xlfn.STDEV.S(files!J8:J9)</f>
-        <v>1.8505396788754985E-2</v>
-      </c>
-      <c r="E5" s="2">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E5" s="2" t="e">
         <f>AVERAGE(files!M8:M9)</f>
-        <v>0.99441688424717145</v>
-      </c>
-      <c r="F5" s="2">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F5" s="2" t="e">
         <f>_xlfn.STDEV.S(files!M8:M9)</f>
-        <v>3.1816728100387383E-3</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="2">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2" t="e">
         <f>AVERAGE(files!J10:J11)</f>
-        <v>0.81619036372224851</v>
-      </c>
-      <c r="C6" s="2">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C6" s="2" t="e">
         <f>_xlfn.STDEV.S(files!J10:J11)</f>
-        <v>1.6116155971776527E-2</v>
-      </c>
-      <c r="E6" s="2">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E6" s="2" t="e">
         <f>AVERAGE(files!M10:M11)</f>
-        <v>0.98451818611242325</v>
-      </c>
-      <c r="F6" s="2">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F6" s="2" t="e">
         <f>_xlfn.STDEV.S(files!M10:M11)</f>
-        <v>7.3649997757030579E-3</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="2">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2" t="e">
         <f>AVERAGE(files!J12:J13)</f>
-        <v>0.74210418878092588</v>
-      </c>
-      <c r="C7" s="2">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C7" s="2" t="e">
         <f>_xlfn.STDEV.S(files!J12:J13)</f>
-        <v>0.10098803551672987</v>
-      </c>
-      <c r="E7" s="2">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E7" s="2" t="e">
         <f>AVERAGE(files!M12:M13)</f>
-        <v>0.98736016983751118</v>
-      </c>
-      <c r="F7" s="2">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F7" s="2" t="e">
         <f>_xlfn.STDEV.S(files!M12:M13)</f>
-        <v>5.0577736614633578E-3</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="2">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="e">
         <f>AVERAGE(files!J14:J14)</f>
-        <v>0.66037735849056611</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="C8" s="2" t="e">
         <f>_xlfn.STDEV.S(files!J14:J14)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="2" t="e">
         <f>AVERAGE(files!M14:M14)</f>
-        <v>0.99419448476052252</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F8" s="2" t="e">
         <f>_xlfn.STDEV.S(files!M14:M14)</f>

</xml_diff>